<commit_message>
t data new push
</commit_message>
<xml_diff>
--- a/T_data.xlsx
+++ b/T_data.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20370"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20371"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\data\odps_clt_release_64\bin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\20201116\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{9D87051F-6E15-4924-838C-162569321811}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EEB7B90A-8AE4-40E6-BF47-2299E4B34BB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12132" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>买入价</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -89,11 +90,15 @@
     <t>600529</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
+  <si>
+    <t>603733</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
@@ -777,16 +782,10 @@
   </cellStyles>
   <dxfs count="12">
     <dxf>
-      <numFmt numFmtId="176" formatCode="0.00_ "/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="176" formatCode="0.00_ "/>
@@ -798,10 +797,30 @@
       <numFmt numFmtId="176" formatCode="0.00_ "/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="176" formatCode="0.00_ "/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode="0.00_ "/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="double">
+          <color rgb="FF3F3F3F"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="double">
+          <color rgb="FF3F3F3F"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -813,20 +832,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="double">
-          <color rgb="FF3F3F3F"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="double">
-          <color rgb="FF3F3F3F"/>
-        </top>
       </border>
     </dxf>
   </dxfs>
@@ -843,33 +848,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:N33" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="11" headerRowCellStyle="检查单元格">
-  <autoFilter ref="A1:N33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表2" displayName="表2" ref="A1:N33" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" headerRowCellStyle="检查单元格">
+  <autoFilter ref="A1:N33" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="14">
-    <tableColumn id="1" name="买入日期"/>
-    <tableColumn id="2" name="总资金" dataDxfId="4"/>
-    <tableColumn id="3" name="操作代码" dataDxfId="8"/>
-    <tableColumn id="4" name="买入价"/>
-    <tableColumn id="5" name="买入数量"/>
-    <tableColumn id="11" name="买入手续费" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="买入日期"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="总资金" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="操作代码" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="买入价"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="买入数量"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="买入手续费" dataDxfId="6">
       <calculatedColumnFormula>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="卖出日期" dataDxfId="3"/>
-    <tableColumn id="6" name="卖出价"/>
-    <tableColumn id="7" name="卖出数量"/>
-    <tableColumn id="12" name="卖出手续费" dataDxfId="6">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="卖出日期" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="卖出价"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="卖出数量"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="卖出手续费" dataDxfId="4">
       <calculatedColumnFormula>IF(表2[[#This Row],[卖出数量]]&gt;0,IF(表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]*0.00013&lt;5,5,表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]*0.00013) + 表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]*0.00102,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="结余资金" dataDxfId="5">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="结余资金" dataDxfId="3">
       <calculatedColumnFormula>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="当前收益" dataDxfId="0">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="当前收益" dataDxfId="2">
       <calculatedColumnFormula>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="当前收益率" dataDxfId="2">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="当前收益率" dataDxfId="1">
       <calculatedColumnFormula>表2[[#This Row],[当前收益]]/表2[[#This Row],[总资金]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="累计收益率" dataDxfId="1">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="累计收益率" dataDxfId="0">
       <calculatedColumnFormula>(表2[[#This Row],[结余资金]]-20000)/20000</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1173,30 +1178,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D38" sqref="D38"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.25" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.25" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="10.21875" customWidth="1"/>
     <col min="6" max="6" width="13" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" style="8" customWidth="1"/>
-    <col min="9" max="9" width="10.25" customWidth="1"/>
+    <col min="9" max="9" width="10.21875" customWidth="1"/>
     <col min="10" max="10" width="13" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.25" style="6" customWidth="1"/>
-    <col min="12" max="12" width="9" style="6"/>
+    <col min="11" max="11" width="10.21875" style="6" customWidth="1"/>
+    <col min="12" max="12" width="11.77734375" style="6" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="13" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -1240,7 +1245,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20210201</v>
       </c>
@@ -1290,7 +1295,7 @@
         <v>2.8167562000000181E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20210202</v>
       </c>
@@ -1341,7 +1346,7 @@
         <v>6.2373828000000138E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20210203</v>
       </c>
@@ -1362,97 +1367,139 @@
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
         <v>5.3810000000000002</v>
       </c>
+      <c r="G4" s="8">
+        <v>20210210</v>
+      </c>
       <c r="H4">
-        <v>38.64</v>
+        <v>40.35</v>
       </c>
       <c r="I4">
         <v>500</v>
       </c>
       <c r="J4" s="6">
         <f>IF(表2[[#This Row],[卖出数量]]&gt;0,IF(表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]*0.00013&lt;5,5,表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]*0.00013) + 表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]*0.00102,0)</f>
-        <v>24.706400000000002</v>
+        <v>25.578500000000002</v>
       </c>
       <c r="K4" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>21487.389160000002</v>
+        <v>22341.517060000002</v>
       </c>
       <c r="L4" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
-        <v>239.91259999999966</v>
+        <v>1094.0404999999992</v>
       </c>
       <c r="M4" s="10">
         <f>表2[[#This Row],[当前收益]]/表2[[#This Row],[总资金]]</f>
-        <v>1.1291345554495326E-2</v>
+        <v>5.1490373311417786E-2</v>
       </c>
       <c r="N4" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>7.4369458000000124E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.11707585300000009</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>20210210</v>
+      </c>
       <c r="B5" s="6">
         <f t="shared" si="0"/>
-        <v>21487.389160000002</v>
+        <v>22341.517060000002</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5">
+        <v>22.97</v>
+      </c>
+      <c r="E5">
+        <v>900</v>
       </c>
       <c r="F5" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
-        <v>0</v>
+        <v>5.4134599999999997</v>
+      </c>
+      <c r="G5" s="8">
+        <v>20210218</v>
+      </c>
+      <c r="H5">
+        <v>24.31</v>
+      </c>
+      <c r="I5">
+        <v>900</v>
       </c>
       <c r="J5" s="6">
         <f>IF(表2[[#This Row],[卖出数量]]&gt;0,IF(表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]*0.00013&lt;5,5,表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]*0.00013) + 表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]*0.00102,0)</f>
-        <v>0</v>
+        <v>27.316580000000002</v>
       </c>
       <c r="K5" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>21487.389160000002</v>
+        <v>23514.787020000003</v>
       </c>
       <c r="L5" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
-        <v>0</v>
+        <v>1173.2699600000014</v>
       </c>
       <c r="M5" s="10">
         <f>表2[[#This Row],[当前收益]]/表2[[#This Row],[总资金]]</f>
-        <v>0</v>
+        <v>5.251523237428718E-2</v>
       </c>
       <c r="N5" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>7.4369458000000124E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.17573935100000018</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>20210218</v>
+      </c>
       <c r="B6" s="6">
         <f t="shared" si="0"/>
-        <v>21487.389160000002</v>
+        <v>23514.787020000003</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>92.15</v>
+      </c>
+      <c r="E6">
+        <v>200</v>
       </c>
       <c r="F6" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
-        <v>0</v>
+        <v>5.3685999999999998</v>
+      </c>
+      <c r="H6">
+        <v>93.3</v>
+      </c>
+      <c r="I6">
+        <v>200</v>
       </c>
       <c r="J6" s="6">
         <f>IF(表2[[#This Row],[卖出数量]]&gt;0,IF(表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]*0.00013&lt;5,5,表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]*0.00013) + 表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]*0.00102,0)</f>
-        <v>0</v>
+        <v>24.033200000000001</v>
       </c>
       <c r="K6" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="L6" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
-        <v>0</v>
+        <v>200.59819999999672</v>
       </c>
       <c r="M6" s="10">
         <f>表2[[#This Row],[当前收益]]/表2[[#This Row],[总资金]]</f>
-        <v>0</v>
+        <v>8.530725786688273E-3</v>
       </c>
       <c r="N6" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>7.4369458000000124E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.18576926100000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" s="6">
         <f t="shared" si="0"/>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="F7" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1464,7 +1511,7 @@
       </c>
       <c r="K7" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="L7" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1476,13 +1523,13 @@
       </c>
       <c r="N7" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>7.4369458000000124E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.18576926100000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="6">
         <f t="shared" si="0"/>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="F8" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1494,7 +1541,7 @@
       </c>
       <c r="K8" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="L8" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1506,13 +1553,13 @@
       </c>
       <c r="N8" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>7.4369458000000124E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.18576926100000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
         <f t="shared" si="0"/>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="F9" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1524,7 +1571,7 @@
       </c>
       <c r="K9" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="L9" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1536,13 +1583,13 @@
       </c>
       <c r="N9" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>7.4369458000000124E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.18576926100000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" s="6">
         <f t="shared" si="0"/>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="F10" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1554,7 +1601,7 @@
       </c>
       <c r="K10" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="L10" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1566,13 +1613,13 @@
       </c>
       <c r="N10" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>7.4369458000000124E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.18576926100000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <f t="shared" si="0"/>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="F11" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1584,7 +1631,7 @@
       </c>
       <c r="K11" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="L11" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1596,13 +1643,13 @@
       </c>
       <c r="N11" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>7.4369458000000124E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.18576926100000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
         <f t="shared" si="0"/>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="F12" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1614,7 +1661,7 @@
       </c>
       <c r="K12" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="L12" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1626,13 +1673,13 @@
       </c>
       <c r="N12" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>7.4369458000000124E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.18576926100000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" s="6">
         <f t="shared" si="0"/>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="F13" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1644,7 +1691,7 @@
       </c>
       <c r="K13" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="L13" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1656,13 +1703,13 @@
       </c>
       <c r="N13" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>7.4369458000000124E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.18576926100000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" s="6">
         <f t="shared" si="0"/>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="F14" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1674,7 +1721,7 @@
       </c>
       <c r="K14" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="L14" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1686,13 +1733,13 @@
       </c>
       <c r="N14" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>7.4369458000000124E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.18576926100000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" s="6">
         <f t="shared" si="0"/>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="F15" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1704,7 +1751,7 @@
       </c>
       <c r="K15" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="L15" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1716,13 +1763,13 @@
       </c>
       <c r="N15" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>7.4369458000000124E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.18576926100000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" s="6">
         <f t="shared" si="0"/>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="F16" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1734,7 +1781,7 @@
       </c>
       <c r="K16" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="L16" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1746,13 +1793,13 @@
       </c>
       <c r="N16" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>7.4369458000000124E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
+        <v>0.18576926100000002</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="6">
         <f t="shared" si="0"/>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="F17" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1764,7 +1811,7 @@
       </c>
       <c r="K17" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="L17" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1776,13 +1823,13 @@
       </c>
       <c r="N17" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>7.4369458000000124E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
+        <v>0.18576926100000002</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="6">
         <f t="shared" si="0"/>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="F18" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1794,7 +1841,7 @@
       </c>
       <c r="K18" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="L18" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1806,13 +1853,13 @@
       </c>
       <c r="N18" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>7.4369458000000124E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
+        <v>0.18576926100000002</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="6">
         <f t="shared" si="0"/>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="F19" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1824,7 +1871,7 @@
       </c>
       <c r="K19" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="L19" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1836,13 +1883,13 @@
       </c>
       <c r="N19" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>7.4369458000000124E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
+        <v>0.18576926100000002</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="6">
         <f t="shared" si="0"/>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="F20" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1854,7 +1901,7 @@
       </c>
       <c r="K20" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="L20" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1866,13 +1913,13 @@
       </c>
       <c r="N20" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>7.4369458000000124E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
+        <v>0.18576926100000002</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="6">
         <f t="shared" si="0"/>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="F21" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1884,7 +1931,7 @@
       </c>
       <c r="K21" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="L21" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1896,13 +1943,13 @@
       </c>
       <c r="N21" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>7.4369458000000124E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
+        <v>0.18576926100000002</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="6">
         <f t="shared" si="0"/>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="F22" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1914,7 +1961,7 @@
       </c>
       <c r="K22" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="L22" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1926,13 +1973,13 @@
       </c>
       <c r="N22" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>7.4369458000000124E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
+        <v>0.18576926100000002</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="6">
         <f t="shared" si="0"/>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="F23" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1944,7 +1991,7 @@
       </c>
       <c r="K23" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="L23" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1956,13 +2003,13 @@
       </c>
       <c r="N23" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>7.4369458000000124E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
+        <v>0.18576926100000002</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="6">
         <f t="shared" si="0"/>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="F24" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1974,7 +2021,7 @@
       </c>
       <c r="K24" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="L24" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1986,13 +2033,13 @@
       </c>
       <c r="N24" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>7.4369458000000124E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
+        <v>0.18576926100000002</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="6">
         <f t="shared" si="0"/>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="F25" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -2004,7 +2051,7 @@
       </c>
       <c r="K25" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="L25" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -2016,13 +2063,13 @@
       </c>
       <c r="N25" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>7.4369458000000124E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
+        <v>0.18576926100000002</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="6">
         <f t="shared" si="0"/>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="F26" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -2034,7 +2081,7 @@
       </c>
       <c r="K26" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="L26" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -2046,13 +2093,13 @@
       </c>
       <c r="N26" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>7.4369458000000124E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
+        <v>0.18576926100000002</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="6">
         <f t="shared" si="0"/>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="F27" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -2064,7 +2111,7 @@
       </c>
       <c r="K27" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="L27" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -2076,13 +2123,13 @@
       </c>
       <c r="N27" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>7.4369458000000124E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
+        <v>0.18576926100000002</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="6">
         <f t="shared" si="0"/>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="F28" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -2094,7 +2141,7 @@
       </c>
       <c r="K28" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="L28" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -2106,13 +2153,13 @@
       </c>
       <c r="N28" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>7.4369458000000124E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
+        <v>0.18576926100000002</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="6">
         <f t="shared" si="0"/>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="F29" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -2124,7 +2171,7 @@
       </c>
       <c r="K29" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="L29" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -2136,13 +2183,13 @@
       </c>
       <c r="N29" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>7.4369458000000124E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.2">
+        <v>0.18576926100000002</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="6">
         <f t="shared" si="0"/>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="F30" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -2154,7 +2201,7 @@
       </c>
       <c r="K30" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="L30" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -2166,13 +2213,13 @@
       </c>
       <c r="N30" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>7.4369458000000124E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.2">
+        <v>0.18576926100000002</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" s="6">
         <f t="shared" si="0"/>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="F31" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -2184,7 +2231,7 @@
       </c>
       <c r="K31" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="L31" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -2196,13 +2243,13 @@
       </c>
       <c r="N31" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>7.4369458000000124E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.2">
+        <v>0.18576926100000002</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" s="6">
         <f t="shared" si="0"/>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="F32" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -2214,7 +2261,7 @@
       </c>
       <c r="K32" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="L32" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -2226,13 +2273,13 @@
       </c>
       <c r="N32" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>7.4369458000000124E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.2">
+        <v>0.18576926100000002</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" s="6">
         <f t="shared" si="0"/>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="F33" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -2244,7 +2291,7 @@
       </c>
       <c r="K33" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>21487.389160000002</v>
+        <v>23715.38522</v>
       </c>
       <c r="L33" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -2256,14 +2303,15 @@
       </c>
       <c r="N33" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>7.4369458000000124E-2</v>
+        <v>0.18576926100000002</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
commit from my work computer
</commit_message>
<xml_diff>
--- a/T_data.xlsx
+++ b/T_data.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20371"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20370"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\20201116\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\t\Git\20201116\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EEB7B90A-8AE4-40E6-BF47-2299E4B34BB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4762DE6E-CE3C-48B7-BEAD-2C7A69AF0D2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12132" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1183,25 +1182,25 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.21875" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.25" style="4" customWidth="1"/>
+    <col min="5" max="5" width="10.25" customWidth="1"/>
     <col min="6" max="6" width="13" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" style="8" customWidth="1"/>
-    <col min="9" max="9" width="10.21875" customWidth="1"/>
+    <col min="9" max="9" width="10.25" customWidth="1"/>
     <col min="10" max="10" width="13" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.21875" style="6" customWidth="1"/>
-    <col min="12" max="12" width="11.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.25" style="6" customWidth="1"/>
+    <col min="12" max="12" width="11.75" style="6" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="13" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -1245,7 +1244,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>20210201</v>
       </c>
@@ -1295,7 +1294,7 @@
         <v>2.8167562000000181E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>20210202</v>
       </c>
@@ -1346,7 +1345,7 @@
         <v>6.2373828000000138E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>20210203</v>
       </c>
@@ -1397,7 +1396,7 @@
         <v>0.11707585300000009</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>20210210</v>
       </c>
@@ -1448,7 +1447,7 @@
         <v>0.17573935100000018</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>20210218</v>
       </c>
@@ -1470,36 +1469,36 @@
         <v>5.3685999999999998</v>
       </c>
       <c r="H6">
-        <v>93.3</v>
+        <v>85</v>
       </c>
       <c r="I6">
         <v>200</v>
       </c>
       <c r="J6" s="6">
         <f>IF(表2[[#This Row],[卖出数量]]&gt;0,IF(表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]*0.00013&lt;5,5,表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]*0.00013) + 表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]*0.00102,0)</f>
-        <v>24.033200000000001</v>
+        <v>22.34</v>
       </c>
       <c r="K6" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="L6" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
-        <v>200.59819999999672</v>
+        <v>-1457.7086000000018</v>
       </c>
       <c r="M6" s="10">
         <f>表2[[#This Row],[当前收益]]/表2[[#This Row],[总资金]]</f>
-        <v>8.530725786688273E-3</v>
+        <v>-6.1991146199205573E-2</v>
       </c>
       <c r="N6" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>0.18576926100000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0.10285392100000008</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B7" s="6">
         <f t="shared" si="0"/>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="F7" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1511,7 +1510,7 @@
       </c>
       <c r="K7" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="L7" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1523,13 +1522,13 @@
       </c>
       <c r="N7" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>0.18576926100000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0.10285392100000008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B8" s="6">
         <f t="shared" si="0"/>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="F8" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1541,7 +1540,7 @@
       </c>
       <c r="K8" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="L8" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1553,13 +1552,13 @@
       </c>
       <c r="N8" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>0.18576926100000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0.10285392100000008</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B9" s="6">
         <f t="shared" si="0"/>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="F9" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1571,7 +1570,7 @@
       </c>
       <c r="K9" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="L9" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1583,13 +1582,13 @@
       </c>
       <c r="N9" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>0.18576926100000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0.10285392100000008</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B10" s="6">
         <f t="shared" si="0"/>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="F10" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1601,7 +1600,7 @@
       </c>
       <c r="K10" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="L10" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1613,13 +1612,13 @@
       </c>
       <c r="N10" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>0.18576926100000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0.10285392100000008</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B11" s="6">
         <f t="shared" si="0"/>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="F11" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1631,7 +1630,7 @@
       </c>
       <c r="K11" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="L11" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1643,13 +1642,13 @@
       </c>
       <c r="N11" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>0.18576926100000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0.10285392100000008</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B12" s="6">
         <f t="shared" si="0"/>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="F12" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1661,7 +1660,7 @@
       </c>
       <c r="K12" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="L12" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1673,13 +1672,13 @@
       </c>
       <c r="N12" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>0.18576926100000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0.10285392100000008</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B13" s="6">
         <f t="shared" si="0"/>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="F13" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1691,7 +1690,7 @@
       </c>
       <c r="K13" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="L13" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1703,13 +1702,13 @@
       </c>
       <c r="N13" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>0.18576926100000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0.10285392100000008</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B14" s="6">
         <f t="shared" si="0"/>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="F14" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1721,7 +1720,7 @@
       </c>
       <c r="K14" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="L14" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1733,13 +1732,13 @@
       </c>
       <c r="N14" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>0.18576926100000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0.10285392100000008</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B15" s="6">
         <f t="shared" si="0"/>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="F15" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1751,7 +1750,7 @@
       </c>
       <c r="K15" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="L15" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1763,13 +1762,13 @@
       </c>
       <c r="N15" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>0.18576926100000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0.10285392100000008</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B16" s="6">
         <f t="shared" si="0"/>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="F16" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1781,7 +1780,7 @@
       </c>
       <c r="K16" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="L16" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1793,13 +1792,13 @@
       </c>
       <c r="N16" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>0.18576926100000002</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.10285392100000008</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B17" s="6">
         <f t="shared" si="0"/>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="F17" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1811,7 +1810,7 @@
       </c>
       <c r="K17" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="L17" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1823,13 +1822,13 @@
       </c>
       <c r="N17" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>0.18576926100000002</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.10285392100000008</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B18" s="6">
         <f t="shared" si="0"/>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="F18" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1841,7 +1840,7 @@
       </c>
       <c r="K18" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="L18" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1853,13 +1852,13 @@
       </c>
       <c r="N18" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>0.18576926100000002</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.10285392100000008</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B19" s="6">
         <f t="shared" si="0"/>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="F19" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1871,7 +1870,7 @@
       </c>
       <c r="K19" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="L19" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1883,13 +1882,13 @@
       </c>
       <c r="N19" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>0.18576926100000002</v>
-      </c>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.10285392100000008</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B20" s="6">
         <f t="shared" si="0"/>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="F20" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1901,7 +1900,7 @@
       </c>
       <c r="K20" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="L20" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1913,13 +1912,13 @@
       </c>
       <c r="N20" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>0.18576926100000002</v>
-      </c>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.10285392100000008</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B21" s="6">
         <f t="shared" si="0"/>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="F21" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1931,7 +1930,7 @@
       </c>
       <c r="K21" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="L21" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1943,13 +1942,13 @@
       </c>
       <c r="N21" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>0.18576926100000002</v>
-      </c>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.10285392100000008</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B22" s="6">
         <f t="shared" si="0"/>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="F22" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1961,7 +1960,7 @@
       </c>
       <c r="K22" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="L22" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -1973,13 +1972,13 @@
       </c>
       <c r="N22" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>0.18576926100000002</v>
-      </c>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.10285392100000008</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B23" s="6">
         <f t="shared" si="0"/>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="F23" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -1991,7 +1990,7 @@
       </c>
       <c r="K23" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="L23" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -2003,13 +2002,13 @@
       </c>
       <c r="N23" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>0.18576926100000002</v>
-      </c>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.10285392100000008</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B24" s="6">
         <f t="shared" si="0"/>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="F24" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -2021,7 +2020,7 @@
       </c>
       <c r="K24" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="L24" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -2033,13 +2032,13 @@
       </c>
       <c r="N24" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>0.18576926100000002</v>
-      </c>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.10285392100000008</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B25" s="6">
         <f t="shared" si="0"/>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="F25" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -2051,7 +2050,7 @@
       </c>
       <c r="K25" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="L25" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -2063,13 +2062,13 @@
       </c>
       <c r="N25" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>0.18576926100000002</v>
-      </c>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.10285392100000008</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B26" s="6">
         <f t="shared" si="0"/>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="F26" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -2081,7 +2080,7 @@
       </c>
       <c r="K26" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="L26" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -2093,13 +2092,13 @@
       </c>
       <c r="N26" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>0.18576926100000002</v>
-      </c>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.10285392100000008</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B27" s="6">
         <f t="shared" si="0"/>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="F27" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -2111,7 +2110,7 @@
       </c>
       <c r="K27" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="L27" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -2123,13 +2122,13 @@
       </c>
       <c r="N27" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>0.18576926100000002</v>
-      </c>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.10285392100000008</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B28" s="6">
         <f t="shared" si="0"/>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="F28" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -2141,7 +2140,7 @@
       </c>
       <c r="K28" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="L28" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -2153,13 +2152,13 @@
       </c>
       <c r="N28" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>0.18576926100000002</v>
-      </c>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.10285392100000008</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B29" s="6">
         <f t="shared" si="0"/>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="F29" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -2171,7 +2170,7 @@
       </c>
       <c r="K29" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="L29" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -2183,13 +2182,13 @@
       </c>
       <c r="N29" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>0.18576926100000002</v>
-      </c>
-    </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.10285392100000008</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B30" s="6">
         <f t="shared" si="0"/>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="F30" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -2201,7 +2200,7 @@
       </c>
       <c r="K30" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="L30" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -2213,13 +2212,13 @@
       </c>
       <c r="N30" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>0.18576926100000002</v>
-      </c>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.10285392100000008</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B31" s="6">
         <f t="shared" si="0"/>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="F31" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -2231,7 +2230,7 @@
       </c>
       <c r="K31" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="L31" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -2243,13 +2242,13 @@
       </c>
       <c r="N31" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>0.18576926100000002</v>
-      </c>
-    </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.10285392100000008</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B32" s="6">
         <f t="shared" si="0"/>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="F32" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -2261,7 +2260,7 @@
       </c>
       <c r="K32" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="L32" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -2273,13 +2272,13 @@
       </c>
       <c r="N32" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>0.18576926100000002</v>
-      </c>
-    </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.10285392100000008</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B33" s="6">
         <f t="shared" si="0"/>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="F33" s="6">
         <f>IF(表2[[#This Row],[买入数量]]&gt;0,IF(表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013&lt;5,5,表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00013) +表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]*0.00002,0)</f>
@@ -2291,7 +2290,7 @@
       </c>
       <c r="K33" s="6">
         <f>表2[[#This Row],[总资金]]-表2[[#This Row],[买入价]]*表2[[#This Row],[买入数量]]+表2[[#This Row],[卖出价]]*表2[[#This Row],[卖出数量]]-表2[[#This Row],[买入手续费]]-表2[[#This Row],[卖出手续费]]</f>
-        <v>23715.38522</v>
+        <v>22057.078420000002</v>
       </c>
       <c r="L33" s="6">
         <f>表2[[#This Row],[结余资金]]-表2[[#This Row],[总资金]]</f>
@@ -2303,7 +2302,7 @@
       </c>
       <c r="N33" s="10">
         <f>(表2[[#This Row],[结余资金]]-20000)/20000</f>
-        <v>0.18576926100000002</v>
+        <v>0.10285392100000008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>